<commit_message>
Initial cut at MHD submission validator
--HG--
branch : feature/simulator
</commit_message>
<xml_diff>
--- a/mhd/validation.xlsx
+++ b/mhd/validation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="0" windowWidth="9080" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28080" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="127">
   <si>
     <t>DocumentEntry.author</t>
   </si>
@@ -103,13 +103,312 @@
   </si>
   <si>
     <t>DocumentEntry.URI</t>
+  </si>
+  <si>
+    <t>attribute</t>
+  </si>
+  <si>
+    <t>element name = status</t>
+  </si>
+  <si>
+    <t>element name = coding</t>
+  </si>
+  <si>
+    <t>coding</t>
+  </si>
+  <si>
+    <t>element name = system</t>
+  </si>
+  <si>
+    <t>attribute name = value</t>
+  </si>
+  <si>
+    <t>element name = code</t>
+  </si>
+  <si>
+    <t>element name = display</t>
+  </si>
+  <si>
+    <t>subjectReference.startsWith('#')</t>
+  </si>
+  <si>
+    <t>thisPatient.size() == 1</t>
+  </si>
+  <si>
+    <t>References contained Patient</t>
+  </si>
+  <si>
+    <t>def patients = dr.contained.Patient</t>
+  </si>
+  <si>
+    <t>patients.each { patient -&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   patient.identifier.system.@value.text().startsWith('urn:oid')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   patient.identifier.value.@value.text() != ''</t>
+  </si>
+  <si>
+    <t>Single subject block exists</t>
+  </si>
+  <si>
+    <t>All contained Patients properly formatted</t>
+  </si>
+  <si>
+    <t>def mimeTypes = dr.mimeType</t>
+  </si>
+  <si>
+    <t>mimeTypes.size() == 1</t>
+  </si>
+  <si>
+    <t>mimeTypes[0].@value.text()  != ''</t>
+  </si>
+  <si>
+    <t>Single mimeType block has value attribute</t>
+  </si>
+  <si>
+    <t>def subjects = dr.subject</t>
+  </si>
+  <si>
+    <t>subjects.size() == 1</t>
+  </si>
+  <si>
+    <t>def subjectReference = subjects[0].reference.@value.text()</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>def authenticators = dr.authenticator</t>
+  </si>
+  <si>
+    <t>authenticators.size() == 1</t>
+  </si>
+  <si>
+    <t>def authenticatorReference = authenticators[0].reference.@value.text()</t>
+  </si>
+  <si>
+    <t>authenticatorReference.startsWith('#')</t>
+  </si>
+  <si>
+    <t>References contained Practitioner</t>
+  </si>
+  <si>
+    <t>def practitioners = dr.contained.Practitioner</t>
+  </si>
+  <si>
+    <t>practitioners.size() == 1</t>
+  </si>
+  <si>
+    <t>Single authenticator block exists, has reference</t>
+  </si>
+  <si>
+    <t>def thisPatient = patients.findAll { it.@id.text() == subjectTab }</t>
+  </si>
+  <si>
+    <t>patients.size() &gt;= 1</t>
+  </si>
+  <si>
+    <t>primaryLanguage block has value attribute</t>
+  </si>
+  <si>
+    <t>dr.primaryLanguage.@value.text() != ''</t>
+  </si>
+  <si>
+    <t>ext def authenticatorTag = authenticatorReference.subStr(1)</t>
+  </si>
+  <si>
+    <t>ext def subjectTag = subjectReference.subStr(1)</t>
+  </si>
+  <si>
+    <t>hcis.size() == 1</t>
+  </si>
+  <si>
+    <t>def hcis = dr.extension.findAll { it.@url.text() == http://ihe.net/fhir/Profile/XDS/extensions#homeCommunityId” }</t>
+  </si>
+  <si>
+    <t>hcis[0].valueString.@value.text().startsWith('urn:oid')</t>
+  </si>
+  <si>
+    <t>homeCommunityId extension is optional</t>
+  </si>
+  <si>
+    <t>thisPractitioner.size() == 1</t>
+  </si>
+  <si>
+    <t>def thisPractitioner = practitioners.findAll { it.@id.text() == authenticatorTag }</t>
+  </si>
+  <si>
+    <t>dr.context.facilityType.coding.size() == 1</t>
+  </si>
+  <si>
+    <t>coding elements present</t>
+  </si>
+  <si>
+    <t>context.facilityType present and coded</t>
+  </si>
+  <si>
+    <t>dr.hash.size() &lt;= 1</t>
+  </si>
+  <si>
+    <t>if (dr.hash.size() == 1) isHex(dr.hash.@value.text())</t>
+  </si>
+  <si>
+    <t>Hash, if present, contains hex value</t>
+  </si>
+  <si>
+    <t>dr.format.@value.text() != ''</t>
+  </si>
+  <si>
+    <t>Format code has value</t>
+  </si>
+  <si>
+    <t>context.event present and coded</t>
+  </si>
+  <si>
+    <t>dr.created.size() == 1</t>
+  </si>
+  <si>
+    <t>isDateTime(dr.created.@value.text())</t>
+  </si>
+  <si>
+    <t>Present and coded</t>
+  </si>
+  <si>
+    <t>0..n</t>
+  </si>
+  <si>
+    <t>Zero or more confidentiality codes present</t>
+  </si>
+  <si>
+    <t>dr.confidentiality.each { verifyCodeStructure(it) }</t>
+  </si>
+  <si>
+    <t>comments.size() &lt;= 1</t>
+  </si>
+  <si>
+    <t>comments.each { it.valueString.@value != '' }</t>
+  </si>
+  <si>
+    <t>Zero or one comment</t>
+  </si>
+  <si>
+    <t>def classCodes = dr.class</t>
+  </si>
+  <si>
+    <t>classCodes.size() &lt;= 1</t>
+  </si>
+  <si>
+    <t>classCodes.each { verifyCodeStructure(it) }</t>
+  </si>
+  <si>
+    <t>Zero or one classCode</t>
+  </si>
+  <si>
+    <t>def statuses = dr.status</t>
+  </si>
+  <si>
+    <t>statuses.size() &lt;= 1</t>
+  </si>
+  <si>
+    <t>def comments = dr.extension.findAll { 
+    it.@url.text() == 'http://ihe.net/fhir/Profile/XDS/extensions#comments'  
+ }</t>
+  </si>
+  <si>
+    <t>statuses[0] in ['current', 'superceeded']</t>
+  </si>
+  <si>
+    <t>0..1</t>
+  </si>
+  <si>
+    <t>1..1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>dr.context.event.each { verifyCodeStructure(it) }</t>
+  </si>
+  <si>
+    <t>def startTime = dr.context.period.start</t>
+  </si>
+  <si>
+    <t>isXmlDateTime(startTime.@value.text())</t>
+  </si>
+  <si>
+    <t>def endTime = dr.context.period.end</t>
+  </si>
+  <si>
+    <t>isXmlDateTime(endTime.@value.text())</t>
+  </si>
+  <si>
+    <t>def extension = dr.extension.find { it.@url.text() == 'http://ihe.net/fhir/Profile/XDS/extensions#sourcePatient'</t>
+  </si>
+  <si>
+    <t>def reference = extension.valueResource.reference.@value.text()</t>
+  </si>
+  <si>
+    <t>reference.startsWith('#')</t>
+  </si>
+  <si>
+    <t>reference = reference.subStr(1)</t>
+  </si>
+  <si>
+    <t>def patient = dr.contained.Patient.find { it.@id.text() == reference }</t>
+  </si>
+  <si>
+    <t>validatePatient(patient)</t>
+  </si>
+  <si>
+    <t>def extension = dr.extension.find { it.@url.text() == 'http://ihe.net/fhir/Profile/XDS/extensions#practiceSettingCode'</t>
+  </si>
+  <si>
+    <t>valueCoding vs coding?</t>
+  </si>
+  <si>
+    <t>validateCoding(extension.valueCoding)</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>FHIR cond</t>
+  </si>
+  <si>
+    <t>XDS cond</t>
+  </si>
+  <si>
+    <t>FHIR card</t>
+  </si>
+  <si>
+    <t>XDS card</t>
+  </si>
+  <si>
+    <t>Stored in Document</t>
+  </si>
+  <si>
+    <t>1..n</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,12 +418,43 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,15 +477,62 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -485,164 +862,862 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A29"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="45.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56" customWidth="1"/>
+    <col min="4" max="4" width="62.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="17">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="17">
-      <c r="A2" s="1" t="s">
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" ht="17">
-      <c r="A3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15">
+      <c r="B4" s="2"/>
+      <c r="D4" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15">
+      <c r="B5" s="2"/>
+      <c r="D5" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15">
+      <c r="B6" s="2"/>
+      <c r="D6" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15">
+      <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" ht="17">
-      <c r="A4" s="1" t="s">
+      <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15">
+      <c r="B8" s="2"/>
+      <c r="D8" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15">
+      <c r="B9" s="2"/>
+      <c r="D9" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15">
+      <c r="B10" s="2"/>
+      <c r="D10" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15">
+      <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" ht="17">
-      <c r="A5" s="1" t="s">
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45">
+      <c r="B12" s="2"/>
+      <c r="D12" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15">
+      <c r="B13" s="2"/>
+      <c r="D13" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15">
+      <c r="B14" s="2"/>
+      <c r="D14" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15">
+      <c r="B15" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" ht="17">
-      <c r="A6" s="1" t="s">
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15">
+      <c r="B16" s="2"/>
+      <c r="D16" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15">
+      <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" ht="17">
-      <c r="A7" s="1" t="s">
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" t="s">
+        <v>101</v>
+      </c>
+      <c r="H17" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15">
+      <c r="B18" s="2"/>
+      <c r="D18" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="15">
+      <c r="B19" s="2"/>
+      <c r="D19" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15">
+      <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" ht="17">
-      <c r="A8" s="1" t="s">
+      <c r="C20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="15">
+      <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" ht="17">
-      <c r="A9" s="1" t="s">
+      <c r="C21" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+      <c r="H21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15">
+      <c r="B22" s="2"/>
+      <c r="D22" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="15">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:8" ht="15">
+      <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" ht="17">
-      <c r="A10" s="1" t="s">
+      <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="15">
+      <c r="B25" s="2"/>
+      <c r="D25" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="15">
+      <c r="B26" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" ht="17">
-      <c r="A11" s="1" t="s">
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" t="s">
+        <v>101</v>
+      </c>
+      <c r="H26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="15">
+      <c r="B27" s="2"/>
+      <c r="D27" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="15">
+      <c r="B28" s="2"/>
+      <c r="D28" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="15">
+      <c r="B29" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" ht="17">
-      <c r="A12" s="1" t="s">
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="15">
+      <c r="B30" s="2"/>
+      <c r="D30" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" ht="15">
+      <c r="B31" s="2"/>
+      <c r="D31" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="15">
+      <c r="B32" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" ht="17">
-      <c r="A13" s="1" t="s">
+      <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="30">
+      <c r="B33" s="2"/>
+      <c r="D33" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="15">
+      <c r="B34" s="2"/>
+      <c r="D34" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="15">
+      <c r="B35" s="2"/>
+      <c r="D35" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="15">
+      <c r="B36" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" ht="17">
-      <c r="A14" s="1" t="s">
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="F36" t="s">
+        <v>100</v>
+      </c>
+      <c r="H36" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" ht="15">
+      <c r="B37" s="2"/>
+      <c r="D37" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="15">
+      <c r="B38" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" ht="17">
-      <c r="A15" s="1" t="s">
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" t="s">
+        <v>99</v>
+      </c>
+      <c r="H38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="15">
+      <c r="B39" s="2"/>
+      <c r="D39" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" ht="15">
+      <c r="B40" s="2"/>
+      <c r="D40" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="15">
+      <c r="B41" s="2"/>
+      <c r="D41" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="15">
+      <c r="B42" s="2"/>
+      <c r="D42" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="15">
+      <c r="B43" s="2"/>
+      <c r="D43" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" ht="15">
+      <c r="B44" s="2"/>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" ht="15">
+      <c r="B45" s="2"/>
+      <c r="D45" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="15">
+      <c r="B46" s="2"/>
+      <c r="D46" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="2:8" ht="30">
+      <c r="B47" s="2"/>
+      <c r="D47" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="15">
+      <c r="B48" s="2"/>
+      <c r="D48" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="2:8" ht="15">
+      <c r="B49" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" ht="17">
-      <c r="A16" s="1" t="s">
+      <c r="C49" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" t="s">
+        <v>100</v>
+      </c>
+      <c r="H49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="15">
+      <c r="B50" s="2"/>
+      <c r="D50" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="15">
+      <c r="B51" s="2"/>
+      <c r="D51" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" ht="15">
+      <c r="B52" s="2"/>
+      <c r="D52" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" ht="15">
+      <c r="B53" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="17">
-      <c r="A17" s="1" t="s">
+      <c r="C53" t="s">
+        <v>43</v>
+      </c>
+      <c r="F53" t="s">
+        <v>100</v>
+      </c>
+      <c r="H53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="15">
+      <c r="B54" s="2"/>
+      <c r="D54" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="15">
+      <c r="B55" s="2"/>
+      <c r="D55" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="15">
+      <c r="B56" s="2"/>
+      <c r="D56" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" ht="15">
+      <c r="B57" s="2"/>
+      <c r="D57" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="15">
+      <c r="B58" s="2"/>
+      <c r="D58" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" ht="15">
+      <c r="B59" s="2"/>
+      <c r="C59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="15">
+      <c r="B60" s="2"/>
+      <c r="D60" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="15">
+      <c r="B61" s="2"/>
+      <c r="D61" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="15">
+      <c r="B62" s="2"/>
+      <c r="D62" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="15">
+      <c r="B63" s="2"/>
+      <c r="D63" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" ht="15">
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="2:8" ht="15">
+      <c r="B65" s="2"/>
+      <c r="C65" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="15">
+      <c r="B66" s="2"/>
+      <c r="D66" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" ht="15">
+      <c r="B67" s="2"/>
+      <c r="D67" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" ht="15">
+      <c r="B68" s="2"/>
+      <c r="D68" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" ht="15">
+      <c r="B69" s="2"/>
+      <c r="D69" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" ht="15">
+      <c r="B70" s="2"/>
+      <c r="D70" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="15">
+      <c r="B71" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="17">
-      <c r="A18" s="1" t="s">
+      <c r="F71" t="s">
+        <v>99</v>
+      </c>
+      <c r="H71" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="15">
+      <c r="B72" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="17">
-      <c r="A19" s="1" t="s">
+      <c r="F72" t="s">
+        <v>99</v>
+      </c>
+      <c r="H72" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" ht="15">
+      <c r="B73" s="2"/>
+      <c r="D73" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" ht="15">
+      <c r="B74" s="2"/>
+      <c r="D74" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" ht="15">
+      <c r="B75" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="17">
-      <c r="A20" s="1" t="s">
+      <c r="F75" t="s">
+        <v>99</v>
+      </c>
+      <c r="H75" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" ht="15">
+      <c r="B76" s="2"/>
+      <c r="D76" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="15">
+      <c r="B77" s="2"/>
+      <c r="D77" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" ht="15">
+      <c r="B78" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" ht="17">
-      <c r="A21" s="1" t="s">
+      <c r="F78" t="s">
+        <v>99</v>
+      </c>
+      <c r="H78" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" ht="15">
+      <c r="B79" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="17">
-      <c r="A22" s="1" t="s">
+      <c r="F79" t="s">
+        <v>99</v>
+      </c>
+      <c r="H79" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" ht="30">
+      <c r="B80" s="2"/>
+      <c r="D80" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" ht="15">
+      <c r="B81" s="2"/>
+      <c r="D81" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" ht="15">
+      <c r="B82" s="2"/>
+      <c r="D82" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" ht="15">
+      <c r="B83" s="2"/>
+      <c r="D83" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" ht="15">
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="2:8" ht="15">
+      <c r="B85" s="2"/>
+      <c r="D85" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" ht="15">
+      <c r="B86" s="2"/>
+      <c r="D86" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" ht="15">
+      <c r="B87" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="17">
-      <c r="A23" s="1" t="s">
+      <c r="F87" t="s">
+        <v>99</v>
+      </c>
+      <c r="H87" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" ht="30">
+      <c r="B88" s="2"/>
+      <c r="D88" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" ht="15">
+      <c r="B89" s="2"/>
+      <c r="D89" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" ht="15">
+      <c r="B90" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" ht="17">
-      <c r="A24" s="1" t="s">
+      <c r="F90" t="s">
+        <v>85</v>
+      </c>
+      <c r="H90" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" ht="15">
+      <c r="B91" s="2"/>
+    </row>
+    <row r="92" spans="2:8" ht="15">
+      <c r="B92" s="2"/>
+    </row>
+    <row r="93" spans="2:8" ht="15">
+      <c r="B93" s="2"/>
+    </row>
+    <row r="94" spans="2:8" ht="15">
+      <c r="B94" s="2"/>
+    </row>
+    <row r="95" spans="2:8" ht="15">
+      <c r="B95" s="2"/>
+    </row>
+    <row r="96" spans="2:8" ht="15">
+      <c r="B96" s="2"/>
+    </row>
+    <row r="97" spans="2:8" ht="15">
+      <c r="B97" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" ht="17">
-      <c r="A25" s="1" t="s">
+      <c r="F97" t="s">
+        <v>99</v>
+      </c>
+      <c r="H97" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="98" spans="2:8" ht="15">
+      <c r="B98" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" ht="17">
-      <c r="A26" s="1" t="s">
+      <c r="F98" t="s">
+        <v>99</v>
+      </c>
+      <c r="H98" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" ht="15">
+      <c r="B99" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" ht="17">
-      <c r="A27" s="1" t="s">
+      <c r="F99" t="s">
+        <v>99</v>
+      </c>
+      <c r="H99" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" ht="15">
+      <c r="B100" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="17">
-      <c r="A28" s="1" t="s">
+      <c r="F100" t="s">
+        <v>100</v>
+      </c>
+      <c r="H100" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" ht="15">
+      <c r="B101" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="17">
-      <c r="A29" s="1" t="s">
-        <v>16</v>
+      <c r="F101" t="s">
+        <v>99</v>
+      </c>
+      <c r="H101" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="102" spans="2:8" ht="15">
+      <c r="B102" s="2"/>
+    </row>
+    <row r="104" spans="2:8">
+      <c r="B104" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C104" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8">
+      <c r="C105" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8">
+      <c r="C106" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8">
+      <c r="C107" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="108" spans="2:8">
+      <c r="C108" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="2:8">
+      <c r="C109" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="2:8">
+      <c r="C110" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Adding to MHD DocumentReference validator
--HG--
branch : feature/simulator
</commit_message>
<xml_diff>
--- a/mhd/validation.xlsx
+++ b/mhd/validation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28080" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="128">
   <si>
     <t>DocumentEntry.author</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>not coded</t>
   </si>
 </sst>
 </file>
@@ -865,8 +868,8 @@
   <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E30" sqref="E30"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1589,6 +1592,9 @@
       <c r="B90" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C90" t="s">
+        <v>127</v>
+      </c>
       <c r="F90" t="s">
         <v>85</v>
       </c>

</xml_diff>